<commit_message>
Adds reception perception profiles for 3 new wrs
</commit_message>
<xml_diff>
--- a/data/Reception_Perception_Rookies.xlsx
+++ b/data/Reception_Perception_Rookies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{059F4665-2EAE-4D67-8888-41E4767B7803}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DD9121-06B2-4180-B237-92D7756981F0}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
+    <workbookView xWindow="-60" yWindow="19830" windowWidth="16200" windowHeight="18030" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Player</t>
   </si>
@@ -270,6 +270,82 @@
 Positives: His zero-drop rate is a significant plus, ensuring he converts catchable targets into receptions (and points). His solid contested catch ability and RAC potential add further value. If a team moves him inside or schemes him effectively against zone, he could find moderate reception volume.
 Negatives: His profound inability to separate against man and press coverage is a major red flag for earning consistent targets, the lifeblood of PPR scoring. If deployed primarily as a traditional X-receiver against NFL corners, his reception volume is likely to be low, capping his fantasy ceiling significantly.
 Overall: Higgins fantasy value appears heavily dependent on his landing spot and role. While his secure hands offer a safe baseline when targeted, his separation issues make him unlikely to be a high-volume receiver unless utilized creatively (e.g., big slot against zone, schemed touches). He profiles as a player whose physical tools might entice teams, but whose on-field production for fantasy might be limited without specific role catering, similar to the concerns surrounding Keon Coleman entering the league.</t>
+  </si>
+  <si>
+    <t>Romeo Doubs</t>
+  </si>
+  <si>
+    <t>Okay, let's break down Elic Ayomanor's profile through our half-point PPR fantasy lens. This is an interesting one, definitely a player with some clear peaks and valleys in his game based on this Reception Perception report.
+Here's the fantasy-focused scouting report on Ayomanor:
+Strengths:
+Man Coverage Dominance: His 70.9% success rate versus man is a big green flag, especially for an X-receiver archetype. He clearly knows how to create separation against single coverage, particularly on those money routes like slants, digs, and posts. This is promising for earning targets and converting them into catches, which gets us that valuable half-point.
+Prototypical X-Receiver Build/Role: He primarily lines up outside and on the line, fitting the traditional 'X' mold. Teams often rely on their X to win one-on-one, aligning with his strength vs. man.
+YAC Potential: Being described as an "underrated tackle-breaker" who breaks contact frequently after the catch is a nice bonus. Those extra yards after the reception can add up, boosting his fantasy score beyond just the catch itself.
+Build-Up Speed: While not explosive off the line, he possesses good long speed (74th percentile 40-yard dash). This gives him the potential to generate chunk plays downfield if he gets a clean release.
+Weaknesses:
+Struggles vs. Press &amp; Zone: This is the major concern. His low success rates against press (64.6%, 35th percentile) and zone (74.6%, 21st percentile) are red flags. Difficulty getting off the line cleanly against physical corners and finding soft spots in zone will limit his ability to consistently demand targets, especially on key outside routes like fades, comebacks, and curls. This caps his volume ceiling, a crucial factor in PPR formats.
+Lack of Initial Burst: The poor 10-yard split confirms what the tape shows – he's not sudden off the line. This contributes to his press struggles and makes it harder to create immediate separation.
+Inconsistent Hands &amp; Drops: A 6.8% drop rate and specific mentions of lapses on open targets and issues securing contested catches (despite good positioning) are significant worries. Drops kill drives and erode QB trust, potentially impacting future targets. Reliability is key in fantasy, especially PPR. Letting contested balls slip despite getting his hands on them is particularly concerning for an X-receiver type often targeted in those situations.
+Development Needed: He's not a polished product. Needs refinement in releases against press, understanding zone nuances, and securing the football consistently.
+Veteran NFL Comparison:
+Romeo Doubs: This comparison feels apt based on the profile. Doubs also came into the league needing refinement, particularly with his hands, but possessed size and the ability to win on certain routes. Like Doubs, Ayomanor might take time to develop into a reliable fantasy starter and may profile more as a solid possession WR2/3 type rather than an elite target hog, especially early on. Both share that potential for inconsistency tied to hands and needing specific routes/coverage matchups to thrive initially.
+Half-PPR Fantasy Summary:
+Ayomanor presents a classic high-variance, Day 2 type profile for fantasy.
+Ceiling: If he lands in an offense that schemes him open, utilizes his strengths on in-breaking routes against man coverage, and he cleans up the drops while improving against press, he could develop into a solid fantasy WR3 with WR2 upside. His size and ability after the catch offer paths to scoring.
+Floor: The significant weaknesses against press/zone and the unreliable hands create a concerning floor. He could struggle to earn consistent targets, becoming a frustrating boom-or-bust fantasy asset heavily dependent on finding the endzone or breaking a long play. In half-PPR, consistent volume is still highly valuable, and his profile suggests that might be a challenge early on.
+Bottom Line: From a fantasy perspective, Ayomanor is a developmental prospect. His ability to beat man coverage gives him a pathway to NFL snaps and targets. However, the significant hurdles against press/zone and the shaky hands make him a risky investment, especially in PPR formats where consistency is prized. He's likely a mid-to-late round rookie pick in dynasty leagues, viewed as a project with upside rather than an immediate impact player. His fantasy value will heavily depend on draft capital, landing spot, and ironing out those key weaknesses. The Romeo Doubs comp suggests patience will be required.</t>
+  </si>
+  <si>
+    <t>Strengths:
+Man &amp; Press Dominator: This is Harris's calling card. High success rates against both man (73.2%, 74th percentile) and press (72.2%, 78th percentile) are exactly what you want from an outside X-receiver. He's physical, uses his hands well, and can get vertical quickly after release. This ability to win one-on-one should earn him opportunities at the next level.
+Vertical Threat &amp; Key Route Proficiency: He lives on the vertical plane, excelling on nines (go routes) and showing fantastic stop-down ability on curls. His success rates on these routes, plus slants, are described as "outrageously high." This suggests he can be a reliable target on the routes he does run well.
+Contested Catch Specialist: A 75% contested catch rate is elite. He tracks the ball well and uses his frame effectively, showing improvement throughout college. This gives him significant touchdown upside in the red zone and on downfield shots.
+Physicality: Fits the "big receiver" mold, is combative, and isn't afraid of hand-fighting. This toughness translates well to beating press and fighting for the ball.
+Weaknesses:
+Zone Coverage Deficiencies: His low success rate vs. zone (75.2%, 24th percentile) is a significant concern for volume potential. He needs to develop a much better feel for finding soft spots, particularly in the intermediate areas. This could limit his quarterback's trust in targeting him consistently against zone looks.
+Limited Route Tree: The report highlights a heavy reliance on screens, curls, and nines (56% combined). While he excels at some of these, the lack of diversity is concerning for early-career impact and limits how consistently he can get open against varied defensive looks. This is more extreme than even Brian Thomas Jr.'s perceived limitation coming out.
+Needs Development: He's not plug-and-play across the full route tree or against all coverages. Significant development is needed in route diversity and zone recognition to become a high-volume receiver.
+Veteran NFL Comparisons:
+Peak Ceiling: DK Metcalf (similar strengths in physicality and vertical ability, though Metcalf is a superior athlete).
+Potential Role/Floor: Alec Pierce (a vertical field-stretcher who excels vs. press but offers limited route diversity and consistency). The hope is Harris offers more consistent impact than Pierce.
+Cautionary Tale: Terrace Marshall (similar Reception Perception profile – strong vs. man, weak vs. zone, excelled on limited routes – but failed to translate). This highlights the risk associated with this type of prospect profile.
+Half-PPR Fantasy Summary:
+Tre Harris profiles as a classic boom-or-bust fantasy receiver early in his career, with his value heavily tied to his specific role and development.
+Upside: His ability to beat press, win deep, and dominate contested catches gives him significant touchdown equity and the potential for week-winning spike weeks. If he lands with a team that needs a vertical X-receiver and utilizes his strengths (curls, nines, maybe slants), he could provide immediate value as a big-play threat. The half-point per reception is less critical for his current archetype, which relies more on chunk plays and TDs than volume.
+Downside: The severe limitations against zone and the narrow route tree make consistent target volume a major question mark. In half-PPR, you still need reliable targets, and he might struggle to provide that week-to-week. He could easily become a volatile fantasy asset, disappearing for stretches if defenses deploy zone coverage effectively or if he doesn't expand his route repertoire quickly. The Terrace Marshall comparison looms large as a potential outcome if he doesn't develop.
+Bottom Line: Harris is an exciting prospect because of his clear strengths in beating man/press coverage and winning contested balls. He fits a valuable NFL archetype. However, for fantasy, especially half-PPR, the lack of polish against zone and the limited route tree make him a risky bet for consistent production early on. He's likely a Day 2 pick (the profile suggests early Round 2) who offers immediate splash-play potential but needs the right offensive scheme and coaching to unlock his full potential and become a reliable fantasy starter. Think of him as a high-upside WR4/5 in rookie drafts with the potential to grow into much more, but also carrying significant bust potential if the weaknesses aren't addressed.</t>
+  </si>
+  <si>
+    <t>Peak - DK Metcalf
+Mid - Alec Pierce
+Low - Terrace Marshall</t>
+  </si>
+  <si>
+    <t>Josh Downs, Tyler Lockett, Ladd McConkey</t>
+  </si>
+  <si>
+    <t>Alright, let's dive into Jaylin Noel from Iowa State. This is the kind of profile that gets me excited when looking for value beyond the top tier. Reception Perception paints a very encouraging picture for his transition to the pros, especially through our half-point PPR lens.
+Here’s the fantasy breakdown for Jaylin Noel:
+Strengths:
+Separation Savvy (Man &amp; Zone): This is where Noel shines. An elite 74.1% success rate vs. man (84th percentile) and a very strong 81.8% vs. zone (64th percentile) show a player who consistently gets open. He's adept at winning on key routes like digs, posts, slants, and flats – the bread-and-butter routes for PPR production. Comparisons to McConkey/Pearsall/Downs in separation ability are high praise.
+Contested Catch Prowess: Despite his 5'10" frame, he boasts an incredible 80% contested catch rate. He plays with a "hulking wideout" mentality, attacks the ball, uses his body well, and secures through contact. This makes him reliable in tight windows and adds red-zone potential.
+Slot Versatility &amp; Mismatch Potential: Primarily a slot receiver (72.5% off LOS), but has experience outside and even in the backfield. This versatility, combined with his route running, can create mismatches for defenses.
+Solid Press Release (for his role): A 55th percentile success rate vs. press (68.4%) is more than adequate for a primary slot receiver and suggests he can handle occasional press looks or even function as a flanker. He has release moves, particularly effective on in-breakers.
+Reliability: His ability to win underneath against zone makes him a reliable target for easy completions (layups), perfect for moving the chains and racking up receptions. His contested catch skill implies strong hands.
+Weaknesses:
+Limited After-the-Catch Threat: This is the main drawback. He's not dynamic with the ball in his hands, going down on first contact frequently (77.8% when in space). Don't expect many extra fantasy points generated via broken tackles; he relies on separation before the catch.
+Specific Route Limitations: Struggles on curls and isn't dominant on nines or outs. These routes often require winning physically on the boundary, where his size can be a disadvantage against bigger corners. His game is tilted more towards breaking routes and working the middle/underneath.
+Needs Minor Refinement: Could improve efficiency in press releases (avoiding extra steps).
+Veteran NFL Comparisons:
+Primary Comp: Josh Downs (excellent separator vs. man, strong at catch point despite size). This is a very positive comp given Downs' effectiveness.
+Archetype/Potential Ceiling: Tyler Lockett (via the Downs comp - smart, reliable, high-volume separator who wins despite size).
+Skill Set Similarity: Ladd McConkey (in terms of route running and obliterating man coverage, though McConkey had other strengths).
+Half-PPR Fantasy Summary:
+Jaylin Noel looks like a potential PPR gem waiting to be drafted, likely on Day 2.
+Potential PPR Machine: His elite separation skills against both man and zone, combined with reliability on underneath and intermediate routes, give him legitimate high-volume target potential from the slot. He's the type of player quarterbacks love – someone who is consistently open. That half-point per reception significantly elevates his fantasy value profile.
+High Floor: Players who separate like this tend to translate well and offer a reliable weekly floor. His contested catch ability adds another layer of reliability.
+Usage/Role: He projects as an immediate contributor in the slot, capable of handling a significant target share. His ability to win vertically from the inside and handle occasional press adds to his value. While the lack of YAC limits massive ceiling plays after the catch, his route running and hands before the catch can lead to big fantasy days through volume and potential TDs (especially given his contested catch skill).
+Bottom Line: Noel profiles as an incredibly safe and potentially high-volume slot receiver at the next level. From a half-PPR standpoint, he's exactly the kind of player you target for consistent production. While he might lack the explosive YAC upside of some other prospects, his ability to get open and catch the football in traffic should make him a reliable fantasy asset, potentially developing into a WR2/3 in PPR formats. He feels like one of the safer bets outside of Round 1, mirroring the Josh Downs trajectory – an underrated prospect poised for immediate impact in the right system. He'll be a favorite target of mine on Day 2 of rookie drafts.</t>
   </si>
 </sst>
 </file>
@@ -327,10 +403,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70176A1-B136-4145-B48A-7863F0F59492}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -933,20 +1005,92 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>48.8</v>
+      </c>
+      <c r="F7">
+        <v>51.2</v>
+      </c>
+      <c r="G7">
+        <v>14.3</v>
+      </c>
+      <c r="H7">
+        <v>6.3</v>
+      </c>
+      <c r="I7">
+        <v>73.2</v>
+      </c>
+      <c r="J7">
+        <v>74</v>
+      </c>
+      <c r="K7">
+        <v>75.2</v>
+      </c>
+      <c r="L7">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <v>72.2</v>
+      </c>
+      <c r="N7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <v>59.9</v>
+      </c>
+      <c r="F8">
+        <v>40.1</v>
+      </c>
+      <c r="G8">
+        <v>21.4</v>
+      </c>
+      <c r="H8">
+        <v>6.6</v>
+      </c>
+      <c r="I8">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="J8">
+        <v>62</v>
+      </c>
+      <c r="K8">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="L8">
+        <v>21</v>
+      </c>
+      <c r="M8">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="N8">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1001,12 +1145,48 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11">
+        <v>47.4</v>
+      </c>
+      <c r="F11">
+        <v>52.6</v>
+      </c>
+      <c r="G11">
+        <v>12.6</v>
+      </c>
+      <c r="H11">
+        <v>4.3</v>
+      </c>
+      <c r="I11">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="J11">
+        <v>84</v>
+      </c>
+      <c r="K11">
+        <v>81.8</v>
+      </c>
+      <c r="L11">
+        <v>64</v>
+      </c>
+      <c r="M11">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="N11">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Removes formatting and changes page length for rookies
</commit_message>
<xml_diff>
--- a/data/Reception_Perception_Rookies.xlsx
+++ b/data/Reception_Perception_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DD9121-06B2-4180-B237-92D7756981F0}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A9CBF7-2CE7-49CF-A757-68AB616426AE}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="19830" windowWidth="16200" windowHeight="18030" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
+    <workbookView xWindow="0" yWindow="19770" windowWidth="16200" windowHeight="18030" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,36 +275,23 @@
     <t>Romeo Doubs</t>
   </si>
   <si>
-    <t>Okay, let's break down Elic Ayomanor's profile through our half-point PPR fantasy lens. This is an interesting one, definitely a player with some clear peaks and valleys in his game based on this Reception Perception report.
-Here's the fantasy-focused scouting report on Ayomanor:
-Strengths:
-Man Coverage Dominance: His 70.9% success rate versus man is a big green flag, especially for an X-receiver archetype. He clearly knows how to create separation against single coverage, particularly on those money routes like slants, digs, and posts. This is promising for earning targets and converting them into catches, which gets us that valuable half-point.
-Prototypical X-Receiver Build/Role: He primarily lines up outside and on the line, fitting the traditional 'X' mold. Teams often rely on their X to win one-on-one, aligning with his strength vs. man.
-YAC Potential: Being described as an "underrated tackle-breaker" who breaks contact frequently after the catch is a nice bonus. Those extra yards after the reception can add up, boosting his fantasy score beyond just the catch itself.
-Build-Up Speed: While not explosive off the line, he possesses good long speed (74th percentile 40-yard dash). This gives him the potential to generate chunk plays downfield if he gets a clean release.
+    <t>Peak - DK Metcalf
+Mid - Alec Pierce
+Low - Terrace Marshall</t>
+  </si>
+  <si>
+    <t>Josh Downs, Tyler Lockett, Ladd McConkey</t>
+  </si>
+  <si>
+    <t>Strengths:
+Man &amp; Press Dominator: This is Harriss calling card. High success rates against both man (73.2%, 74th percentile) and press (72.2%, 78th percentile) are exactly what you want from an outside X-receiver. Hes physical, uses his hands well, and can get vertical quickly after release. This ability to win one-on-one should earn him opportunities at the next level.
+Vertical Threat &amp; Key Route Proficiency: He lives on the vertical plane, excelling on nines (go routes) and showing fantastic stop-down ability on curls. His success rates on these routes, plus slants, are described as outrageously high. This suggests he can be a reliable target on the routes he does run well.
+Contested Catch Specialist: A 75% contested catch rate is elite. He tracks the ball well and uses his frame effectively, showing improvement throughout college. This gives him significant touchdown upside in the red zone and on downfield shots.
+Physicality: Fits the big receiver mold, is combative, and isnt afraid of hand-fighting. This toughness translates well to beating press and fighting for the ball.
 Weaknesses:
-Struggles vs. Press &amp; Zone: This is the major concern. His low success rates against press (64.6%, 35th percentile) and zone (74.6%, 21st percentile) are red flags. Difficulty getting off the line cleanly against physical corners and finding soft spots in zone will limit his ability to consistently demand targets, especially on key outside routes like fades, comebacks, and curls. This caps his volume ceiling, a crucial factor in PPR formats.
-Lack of Initial Burst: The poor 10-yard split confirms what the tape shows – he's not sudden off the line. This contributes to his press struggles and makes it harder to create immediate separation.
-Inconsistent Hands &amp; Drops: A 6.8% drop rate and specific mentions of lapses on open targets and issues securing contested catches (despite good positioning) are significant worries. Drops kill drives and erode QB trust, potentially impacting future targets. Reliability is key in fantasy, especially PPR. Letting contested balls slip despite getting his hands on them is particularly concerning for an X-receiver type often targeted in those situations.
-Development Needed: He's not a polished product. Needs refinement in releases against press, understanding zone nuances, and securing the football consistently.
-Veteran NFL Comparison:
-Romeo Doubs: This comparison feels apt based on the profile. Doubs also came into the league needing refinement, particularly with his hands, but possessed size and the ability to win on certain routes. Like Doubs, Ayomanor might take time to develop into a reliable fantasy starter and may profile more as a solid possession WR2/3 type rather than an elite target hog, especially early on. Both share that potential for inconsistency tied to hands and needing specific routes/coverage matchups to thrive initially.
-Half-PPR Fantasy Summary:
-Ayomanor presents a classic high-variance, Day 2 type profile for fantasy.
-Ceiling: If he lands in an offense that schemes him open, utilizes his strengths on in-breaking routes against man coverage, and he cleans up the drops while improving against press, he could develop into a solid fantasy WR3 with WR2 upside. His size and ability after the catch offer paths to scoring.
-Floor: The significant weaknesses against press/zone and the unreliable hands create a concerning floor. He could struggle to earn consistent targets, becoming a frustrating boom-or-bust fantasy asset heavily dependent on finding the endzone or breaking a long play. In half-PPR, consistent volume is still highly valuable, and his profile suggests that might be a challenge early on.
-Bottom Line: From a fantasy perspective, Ayomanor is a developmental prospect. His ability to beat man coverage gives him a pathway to NFL snaps and targets. However, the significant hurdles against press/zone and the shaky hands make him a risky investment, especially in PPR formats where consistency is prized. He's likely a mid-to-late round rookie pick in dynasty leagues, viewed as a project with upside rather than an immediate impact player. His fantasy value will heavily depend on draft capital, landing spot, and ironing out those key weaknesses. The Romeo Doubs comp suggests patience will be required.</t>
-  </si>
-  <si>
-    <t>Strengths:
-Man &amp; Press Dominator: This is Harris's calling card. High success rates against both man (73.2%, 74th percentile) and press (72.2%, 78th percentile) are exactly what you want from an outside X-receiver. He's physical, uses his hands well, and can get vertical quickly after release. This ability to win one-on-one should earn him opportunities at the next level.
-Vertical Threat &amp; Key Route Proficiency: He lives on the vertical plane, excelling on nines (go routes) and showing fantastic stop-down ability on curls. His success rates on these routes, plus slants, are described as "outrageously high." This suggests he can be a reliable target on the routes he does run well.
-Contested Catch Specialist: A 75% contested catch rate is elite. He tracks the ball well and uses his frame effectively, showing improvement throughout college. This gives him significant touchdown upside in the red zone and on downfield shots.
-Physicality: Fits the "big receiver" mold, is combative, and isn't afraid of hand-fighting. This toughness translates well to beating press and fighting for the ball.
-Weaknesses:
-Zone Coverage Deficiencies: His low success rate vs. zone (75.2%, 24th percentile) is a significant concern for volume potential. He needs to develop a much better feel for finding soft spots, particularly in the intermediate areas. This could limit his quarterback's trust in targeting him consistently against zone looks.
-Limited Route Tree: The report highlights a heavy reliance on screens, curls, and nines (56% combined). While he excels at some of these, the lack of diversity is concerning for early-career impact and limits how consistently he can get open against varied defensive looks. This is more extreme than even Brian Thomas Jr.'s perceived limitation coming out.
-Needs Development: He's not plug-and-play across the full route tree or against all coverages. Significant development is needed in route diversity and zone recognition to become a high-volume receiver.
+Zone Coverage Deficiencies: His low success rate vs. zone (75.2%, 24th percentile) is a significant concern for volume potential. He needs to develop a much better feel for finding soft spots, particularly in the intermediate areas. This could limit his quarterbacks trust in targeting him consistently against zone looks.
+Limited Route Tree: The report highlights a heavy reliance on screens, curls, and nines (56% combined). While he excels at some of these, the lack of diversity is concerning for early-career impact and limits how consistently he can get open against varied defensive looks. This is more extreme than even Brian Thomas Jr.s perceived limitation coming out.
+Needs Development: Hes not plug-and-play across the full route tree or against all coverages. Significant development is needed in route diversity and zone recognition to become a high-volume receiver.
 Veteran NFL Comparisons:
 Peak Ceiling: DK Metcalf (similar strengths in physicality and vertical ability, though Metcalf is a superior athlete).
 Potential Role/Floor: Alec Pierce (a vertical field-stretcher who excels vs. press but offers limited route diversity and consistency). The hope is Harris offers more consistent impact than Pierce.
@@ -312,40 +299,53 @@
 Half-PPR Fantasy Summary:
 Tre Harris profiles as a classic boom-or-bust fantasy receiver early in his career, with his value heavily tied to his specific role and development.
 Upside: His ability to beat press, win deep, and dominate contested catches gives him significant touchdown equity and the potential for week-winning spike weeks. If he lands with a team that needs a vertical X-receiver and utilizes his strengths (curls, nines, maybe slants), he could provide immediate value as a big-play threat. The half-point per reception is less critical for his current archetype, which relies more on chunk plays and TDs than volume.
-Downside: The severe limitations against zone and the narrow route tree make consistent target volume a major question mark. In half-PPR, you still need reliable targets, and he might struggle to provide that week-to-week. He could easily become a volatile fantasy asset, disappearing for stretches if defenses deploy zone coverage effectively or if he doesn't expand his route repertoire quickly. The Terrace Marshall comparison looms large as a potential outcome if he doesn't develop.
-Bottom Line: Harris is an exciting prospect because of his clear strengths in beating man/press coverage and winning contested balls. He fits a valuable NFL archetype. However, for fantasy, especially half-PPR, the lack of polish against zone and the limited route tree make him a risky bet for consistent production early on. He's likely a Day 2 pick (the profile suggests early Round 2) who offers immediate splash-play potential but needs the right offensive scheme and coaching to unlock his full potential and become a reliable fantasy starter. Think of him as a high-upside WR4/5 in rookie drafts with the potential to grow into much more, but also carrying significant bust potential if the weaknesses aren't addressed.</t>
-  </si>
-  <si>
-    <t>Peak - DK Metcalf
-Mid - Alec Pierce
-Low - Terrace Marshall</t>
-  </si>
-  <si>
-    <t>Josh Downs, Tyler Lockett, Ladd McConkey</t>
-  </si>
-  <si>
-    <t>Alright, let's dive into Jaylin Noel from Iowa State. This is the kind of profile that gets me excited when looking for value beyond the top tier. Reception Perception paints a very encouraging picture for his transition to the pros, especially through our half-point PPR lens.
+Downside: The severe limitations against zone and the narrow route tree make consistent target volume a major question mark. In half-PPR, you still need reliable targets, and he might struggle to provide that week-to-week. He could easily become a volatile fantasy asset, disappearing for stretches if defenses deploy zone coverage effectively or if he doesnt expand his route repertoire quickly. The Terrace Marshall comparison looms large as a potential outcome if he doesnt develop.
+Bottom Line: Harris is an exciting prospect because of his clear strengths in beating man/press coverage and winning contested balls. He fits a valuable NFL archetype. However, for fantasy, especially half-PPR, the lack of polish against zone and the limited route tree make him a risky bet for consistent production early on. Hes likely a Day 2 pick (the profile suggests early Round 2) who offers immediate splash-play potential but needs the right offensive scheme and coaching to unlock his full potential and become a reliable fantasy starter. Think of him as a high-upside WR4/5 in rookie drafts with the potential to grow into much more, but also carrying significant bust potential if the weaknesses arent addressed.</t>
+  </si>
+  <si>
+    <t>Okay, lets break down Elic Ayomanors profile through our half-point PPR fantasy lens. This is an interesting one, definitely a player with some clear peaks and valleys in his game based on this Reception Perception report.
+Heres the fantasy-focused scouting report on Ayomanor:
+Strengths:
+Man Coverage Dominance: His 70.9% success rate versus man is a big green flag, especially for an X-receiver archetype. He clearly knows how to create separation against single coverage, particularly on those money routes like slants, digs, and posts. This is promising for earning targets and converting them into catches, which gets us that valuable half-point.
+Prototypical X-Receiver Build/Role: He primarily lines up outside and on the line, fitting the traditional X mold. Teams often rely on their X to win one-on-one, aligning with his strength vs. man.
+YAC Potential: Being described as an underrated tackle-breaker who breaks contact frequently after the catch is a nice bonus. Those extra yards after the reception can add up, boosting his fantasy score beyond just the catch itself.
+Build-Up Speed: While not explosive off the line, he possesses good long speed (74th percentile 40-yard dash). This gives him the potential to generate chunk plays downfield if he gets a clean release.
+Weaknesses:
+Struggles vs. Press &amp; Zone: This is the major concern. His low success rates against press (64.6%, 35th percentile) and zone (74.6%, 21st percentile) are red flags. Difficulty getting off the line cleanly against physical corners and finding soft spots in zone will limit his ability to consistently demand targets, especially on key outside routes like fades, comebacks, and curls. This caps his volume ceiling, a crucial factor in PPR formats.
+Lack of Initial Burst: The poor 10-yard split confirms what the tape shows – hes not sudden off the line. This contributes to his press struggles and makes it harder to create immediate separation.
+Inconsistent Hands &amp; Drops: A 6.8% drop rate and specific mentions of lapses on open targets and issues securing contested catches (despite good positioning) are significant worries. Drops kill drives and erode QB trust, potentially impacting future targets. Reliability is key in fantasy, especially PPR. Letting contested balls slip despite getting his hands on them is particularly concerning for an X-receiver type often targeted in those situations.
+Development Needed: Hes not a polished product. Needs refinement in releases against press, understanding zone nuances, and securing the football consistently.
+Veteran NFL Comparison:
+Romeo Doubs: This comparison feels apt based on the profile. Doubs also came into the league needing refinement, particularly with his hands, but possessed size and the ability to win on certain routes. Like Doubs, Ayomanor might take time to develop into a reliable fantasy starter and may profile more as a solid possession WR2/3 type rather than an elite target hog, especially early on. Both share that potential for inconsistency tied to hands and needing specific routes/coverage matchups to thrive initially.
+Half-PPR Fantasy Summary:
+Ayomanor presents a classic high-variance, Day 2 type profile for fantasy.
+Ceiling: If he lands in an offense that schemes him open, utilizes his strengths on in-breaking routes against man coverage, and he cleans up the drops while improving against press, he could develop into a solid fantasy WR3 with WR2 upside. His size and ability after the catch offer paths to scoring.
+Floor: The significant weaknesses against press/zone and the unreliable hands create a concerning floor. He could struggle to earn consistent targets, becoming a frustrating boom-or-bust fantasy asset heavily dependent on finding the endzone or breaking a long play. In half-PPR, consistent volume is still highly valuable, and his profile suggests that might be a challenge early on.
+Bottom Line: From a fantasy perspective, Ayomanor is a developmental prospect. His ability to beat man coverage gives him a pathway to NFL snaps and targets. However, the significant hurdles against press/zone and the shaky hands make him a risky investment, especially in PPR formats where consistency is prized. Hes likely a mid-to-late round rookie pick in dynasty leagues, viewed as a project with upside rather than an immediate impact player. His fantasy value will heavily depend on draft capital, landing spot, and ironing out those key weaknesses. The Romeo Doubs comp suggests patience will be required.</t>
+  </si>
+  <si>
+    <t>Alright, lets dive into Jaylin Noel from Iowa State. This is the kind of profile that gets me excited when looking for value beyond the top tier. Reception Perception paints a very encouraging picture for his transition to the pros, especially through our half-point PPR lens.
 Here’s the fantasy breakdown for Jaylin Noel:
 Strengths:
-Separation Savvy (Man &amp; Zone): This is where Noel shines. An elite 74.1% success rate vs. man (84th percentile) and a very strong 81.8% vs. zone (64th percentile) show a player who consistently gets open. He's adept at winning on key routes like digs, posts, slants, and flats – the bread-and-butter routes for PPR production. Comparisons to McConkey/Pearsall/Downs in separation ability are high praise.
-Contested Catch Prowess: Despite his 5'10" frame, he boasts an incredible 80% contested catch rate. He plays with a "hulking wideout" mentality, attacks the ball, uses his body well, and secures through contact. This makes him reliable in tight windows and adds red-zone potential.
+Separation Savvy (Man &amp; Zone): This is where Noel shines. An elite 74.1% success rate vs. man (84th percentile) and a very strong 81.8% vs. zone (64th percentile) show a player who consistently gets open. Hes adept at winning on key routes like digs, posts, slants, and flats – the bread-and-butter routes for PPR production. Comparisons to McConkey/Pearsall/Downs in separation ability are high praise.
+Contested Catch Prowess: Despite his 510 frame, he boasts an incredible 80% contested catch rate. He plays with a hulking wideout mentality, attacks the ball, uses his body well, and secures through contact. This makes him reliable in tight windows and adds red-zone potential.
 Slot Versatility &amp; Mismatch Potential: Primarily a slot receiver (72.5% off LOS), but has experience outside and even in the backfield. This versatility, combined with his route running, can create mismatches for defenses.
 Solid Press Release (for his role): A 55th percentile success rate vs. press (68.4%) is more than adequate for a primary slot receiver and suggests he can handle occasional press looks or even function as a flanker. He has release moves, particularly effective on in-breakers.
 Reliability: His ability to win underneath against zone makes him a reliable target for easy completions (layups), perfect for moving the chains and racking up receptions. His contested catch skill implies strong hands.
 Weaknesses:
-Limited After-the-Catch Threat: This is the main drawback. He's not dynamic with the ball in his hands, going down on first contact frequently (77.8% when in space). Don't expect many extra fantasy points generated via broken tackles; he relies on separation before the catch.
-Specific Route Limitations: Struggles on curls and isn't dominant on nines or outs. These routes often require winning physically on the boundary, where his size can be a disadvantage against bigger corners. His game is tilted more towards breaking routes and working the middle/underneath.
+Limited After-the-Catch Threat: This is the main drawback. Hes not dynamic with the ball in his hands, going down on first contact frequently (77.8% when in space). Dont expect many extra fantasy points generated via broken tackles; he relies on separation before the catch.
+Specific Route Limitations: Struggles on curls and isnt dominant on nines or outs. These routes often require winning physically on the boundary, where his size can be a disadvantage against bigger corners. His game is tilted more towards breaking routes and working the middle/underneath.
 Needs Minor Refinement: Could improve efficiency in press releases (avoiding extra steps).
 Veteran NFL Comparisons:
-Primary Comp: Josh Downs (excellent separator vs. man, strong at catch point despite size). This is a very positive comp given Downs' effectiveness.
+Primary Comp: Josh Downs (excellent separator vs. man, strong at catch point despite size). This is a very positive comp given Downs effectiveness.
 Archetype/Potential Ceiling: Tyler Lockett (via the Downs comp - smart, reliable, high-volume separator who wins despite size).
 Skill Set Similarity: Ladd McConkey (in terms of route running and obliterating man coverage, though McConkey had other strengths).
 Half-PPR Fantasy Summary:
 Jaylin Noel looks like a potential PPR gem waiting to be drafted, likely on Day 2.
-Potential PPR Machine: His elite separation skills against both man and zone, combined with reliability on underneath and intermediate routes, give him legitimate high-volume target potential from the slot. He's the type of player quarterbacks love – someone who is consistently open. That half-point per reception significantly elevates his fantasy value profile.
+Potential PPR Machine: His elite separation skills against both man and zone, combined with reliability on underneath and intermediate routes, give him legitimate high-volume target potential from the slot. Hes the type of player quarterbacks love – someone who is consistently open. That half-point per reception significantly elevates his fantasy value profile.
 High Floor: Players who separate like this tend to translate well and offer a reliable weekly floor. His contested catch ability adds another layer of reliability.
 Usage/Role: He projects as an immediate contributor in the slot, capable of handling a significant target share. His ability to win vertically from the inside and handle occasional press adds to his value. While the lack of YAC limits massive ceiling plays after the catch, his route running and hands before the catch can lead to big fantasy days through volume and potential TDs (especially given his contested catch skill).
-Bottom Line: Noel profiles as an incredibly safe and potentially high-volume slot receiver at the next level. From a half-PPR standpoint, he's exactly the kind of player you target for consistent production. While he might lack the explosive YAC upside of some other prospects, his ability to get open and catch the football in traffic should make him a reliable fantasy asset, potentially developing into a WR2/3 in PPR formats. He feels like one of the safer bets outside of Round 1, mirroring the Josh Downs trajectory – an underrated prospect poised for immediate impact in the right system. He'll be a favorite target of mine on Day 2 of rookie drafts.</t>
+Bottom Line: Noel profiles as an incredibly safe and potentially high-volume slot receiver at the next level. From a half-PPR standpoint, hes exactly the kind of player you target for consistent production. While he might lack the explosive YAC upside of some other prospects, his ability to get open and catch the football in traffic should make him a reliable fantasy asset, potentially developing into a WR2/3 in PPR formats. He feels like one of the safer bets outside of Round 1, mirroring the Josh Downs trajectory – an underrated prospect poised for immediate impact in the right system. Hell be a favorite target of mine on Day 2 of rookie drafts.</t>
   </si>
 </sst>
 </file>
@@ -403,6 +403,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70176A1-B136-4145-B48A-7863F0F59492}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>48.8</v>
@@ -1057,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>47</v>
@@ -1156,7 +1160,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>47.4</v>

</xml_diff>

<commit_message>
Updates RP data, adds columns, adds formatting
</commit_message>
<xml_diff>
--- a/data/Reception_Perception_Rookies.xlsx
+++ b/data/Reception_Perception_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A9CBF7-2CE7-49CF-A757-68AB616426AE}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97776D60-3F33-4133-A822-508650AF2741}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="19770" windowWidth="16200" windowHeight="18030" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
+    <workbookView xWindow="38290" yWindow="-12520" windowWidth="21820" windowHeight="38020" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>Player</t>
   </si>
@@ -346,6 +346,60 @@
 High Floor: Players who separate like this tend to translate well and offer a reliable weekly floor. His contested catch ability adds another layer of reliability.
 Usage/Role: He projects as an immediate contributor in the slot, capable of handling a significant target share. His ability to win vertically from the inside and handle occasional press adds to his value. While the lack of YAC limits massive ceiling plays after the catch, his route running and hands before the catch can lead to big fantasy days through volume and potential TDs (especially given his contested catch skill).
 Bottom Line: Noel profiles as an incredibly safe and potentially high-volume slot receiver at the next level. From a half-PPR standpoint, hes exactly the kind of player you target for consistent production. While he might lack the explosive YAC upside of some other prospects, his ability to get open and catch the football in traffic should make him a reliable fantasy asset, potentially developing into a WR2/3 in PPR formats. He feels like one of the safer bets outside of Round 1, mirroring the Josh Downs trajectory – an underrated prospect poised for immediate impact in the right system. Hell be a favorite target of mine on Day 2 of rookie drafts.</t>
+  </si>
+  <si>
+    <t>RP 2021-2025 Rank</t>
+  </si>
+  <si>
+    <t>RP Quick Note</t>
+  </si>
+  <si>
+    <t>RP Definition</t>
+  </si>
+  <si>
+    <t>Clear first rounder</t>
+  </si>
+  <si>
+    <t>Late Round 1 / Early Round 2</t>
+  </si>
+  <si>
+    <t>Top 10 pick / Ready made star</t>
+  </si>
+  <si>
+    <t>Priority Rd 2</t>
+  </si>
+  <si>
+    <t>Straight-line X-receiver who flashes the beginnings of solid route-running. Volatile profile.</t>
+  </si>
+  <si>
+    <t>Don't mind him on Day 2 because he beats man but needs refinement and has hands issues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great hands but struggles to separate vs. man. Much like Coleman, I prefer a power slot future.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot who can play a bit of flanker and specializes in the vertical game. Gets open, wins contested.	</t>
+  </si>
+  <si>
+    <t>Late Round 3  / Early Round 4</t>
+  </si>
+  <si>
+    <t>Good Day 2 Option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic X-receiver who separates well in the intermediate area and is sneaky after the catch.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome RAC player with flashes of man coverage ability. Work ethic concerns but high upside.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe he tops out as a great No. 2 but that's fine. Power slot who can handle outside duties.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical receiver with some excellent grabs in contested situations. Really nice zone routes.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fantastic three-level separator. Elite vs. man, zone, press. Rare catching ability. Will he play WR?	</t>
   </si>
 </sst>
 </file>
@@ -726,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70176A1-B136-4145-B48A-7863F0F59492}">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,15 +791,17 @@
     <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="16.453125" customWidth="1"/>
+    <col min="4" max="7" width="16.08984375" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.453125" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,16 +815,16 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
@@ -777,19 +833,28 @@
         <v>29</v>
       </c>
       <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -802,17 +867,17 @@
       <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2">
         <v>57.2</v>
-      </c>
-      <c r="F2">
-        <v>42.8</v>
-      </c>
-      <c r="G2">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="H2">
-        <v>12.4</v>
       </c>
       <c r="I2">
         <v>70.400000000000006</v>
@@ -821,19 +886,28 @@
         <v>59</v>
       </c>
       <c r="K2">
+        <v>42.8</v>
+      </c>
+      <c r="L2">
         <v>81</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>60</v>
       </c>
-      <c r="M2">
+      <c r="N2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O2">
         <v>73.099999999999994</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q2">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -847,16 +921,16 @@
         <v>41</v>
       </c>
       <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3">
         <v>30.7</v>
-      </c>
-      <c r="F3">
-        <v>69.3</v>
-      </c>
-      <c r="G3">
-        <v>4.2</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
       </c>
       <c r="I3">
         <v>71.2</v>
@@ -865,19 +939,28 @@
         <v>68</v>
       </c>
       <c r="K3">
+        <v>69.3</v>
+      </c>
+      <c r="L3">
         <v>79.400000000000006</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>55</v>
       </c>
-      <c r="M3">
+      <c r="N3">
+        <v>4.2</v>
+      </c>
+      <c r="O3">
         <v>70</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -890,17 +973,17 @@
       <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4">
         <v>44.8</v>
-      </c>
-      <c r="F4">
-        <v>55.2</v>
-      </c>
-      <c r="G4">
-        <v>7.6</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
       </c>
       <c r="I4">
         <v>68.099999999999994</v>
@@ -909,19 +992,28 @@
         <v>42</v>
       </c>
       <c r="K4">
+        <v>55.2</v>
+      </c>
+      <c r="L4">
         <v>83.6</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>82</v>
       </c>
-      <c r="M4">
+      <c r="N4">
+        <v>7.6</v>
+      </c>
+      <c r="O4">
         <v>81.3</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -935,16 +1027,16 @@
         <v>39</v>
       </c>
       <c r="E5">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5">
         <v>43.4</v>
-      </c>
-      <c r="F5">
-        <v>56.6</v>
-      </c>
-      <c r="G5">
-        <v>20.3</v>
-      </c>
-      <c r="H5">
-        <v>4.7</v>
       </c>
       <c r="I5">
         <v>68.5</v>
@@ -953,19 +1045,28 @@
         <v>44</v>
       </c>
       <c r="K5">
+        <v>56.6</v>
+      </c>
+      <c r="L5">
         <v>82.5</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>77</v>
       </c>
-      <c r="M5">
+      <c r="N5">
+        <v>20.3</v>
+      </c>
+      <c r="O5">
         <v>67.400000000000006</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -978,17 +1079,17 @@
       <c r="D6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6">
         <v>44.5</v>
-      </c>
-      <c r="F6">
-        <v>55.5</v>
-      </c>
-      <c r="G6">
-        <v>22.6</v>
-      </c>
-      <c r="H6">
-        <v>9.5</v>
       </c>
       <c r="I6">
         <v>78.599999999999994</v>
@@ -997,19 +1098,28 @@
         <v>92</v>
       </c>
       <c r="K6">
+        <v>55.5</v>
+      </c>
+      <c r="L6">
         <v>87.9</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>97</v>
       </c>
-      <c r="M6">
+      <c r="N6">
+        <v>22.6</v>
+      </c>
+      <c r="O6">
         <v>84.4</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q6">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1022,17 +1132,17 @@
       <c r="D7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7">
         <v>48.8</v>
-      </c>
-      <c r="F7">
-        <v>51.2</v>
-      </c>
-      <c r="G7">
-        <v>14.3</v>
-      </c>
-      <c r="H7">
-        <v>6.3</v>
       </c>
       <c r="I7">
         <v>73.2</v>
@@ -1041,19 +1151,28 @@
         <v>74</v>
       </c>
       <c r="K7">
+        <v>51.2</v>
+      </c>
+      <c r="L7">
         <v>75.2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>24</v>
       </c>
-      <c r="M7">
+      <c r="N7">
+        <v>14.3</v>
+      </c>
+      <c r="O7">
         <v>72.2</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1066,17 +1185,17 @@
       <c r="D8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8">
         <v>59.9</v>
-      </c>
-      <c r="F8">
-        <v>40.1</v>
-      </c>
-      <c r="G8">
-        <v>21.4</v>
-      </c>
-      <c r="H8">
-        <v>6.6</v>
       </c>
       <c r="I8">
         <v>70.900000000000006</v>
@@ -1085,19 +1204,28 @@
         <v>62</v>
       </c>
       <c r="K8">
+        <v>40.1</v>
+      </c>
+      <c r="L8">
         <v>74.599999999999994</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>21</v>
       </c>
-      <c r="M8">
+      <c r="N8">
+        <v>21.4</v>
+      </c>
+      <c r="O8">
         <v>64.599999999999994</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1118,17 +1246,17 @@
       <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
+        <v>52</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10">
         <v>58.4</v>
-      </c>
-      <c r="F10">
-        <v>41.6</v>
-      </c>
-      <c r="G10">
-        <v>27.1</v>
-      </c>
-      <c r="H10">
-        <v>1.9</v>
       </c>
       <c r="I10">
         <v>58.6</v>
@@ -1137,19 +1265,28 @@
         <v>15</v>
       </c>
       <c r="K10">
+        <v>41.6</v>
+      </c>
+      <c r="L10">
         <v>78.599999999999994</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>46</v>
       </c>
-      <c r="M10">
+      <c r="N10">
+        <v>27.1</v>
+      </c>
+      <c r="O10">
         <v>50.7</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="Q10">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1162,17 +1299,17 @@
       <c r="D11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11">
         <v>47.4</v>
-      </c>
-      <c r="F11">
-        <v>52.6</v>
-      </c>
-      <c r="G11">
-        <v>12.6</v>
-      </c>
-      <c r="H11">
-        <v>4.3</v>
       </c>
       <c r="I11">
         <v>74.099999999999994</v>
@@ -1181,19 +1318,28 @@
         <v>84</v>
       </c>
       <c r="K11">
+        <v>52.6</v>
+      </c>
+      <c r="L11">
         <v>81.8</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>64</v>
       </c>
-      <c r="M11">
+      <c r="N11">
+        <v>12.6</v>
+      </c>
+      <c r="O11">
         <v>68.400000000000006</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Q11">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1217,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1225,7 +1371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1241,7 +1387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1249,7 +1395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1257,7 +1403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1265,7 +1411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1273,40 +1419,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G31" s="1"/>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G35" s="1"/>
-    </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G39" s="1"/>
-    </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G43" s="1"/>
-    </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G47" s="2"/>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" s="2"/>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" s="1"/>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" s="1"/>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" s="1"/>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G67" s="2"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N35" s="1"/>
+    </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N39" s="1"/>
+    </row>
+    <row r="43" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N43" s="1"/>
+    </row>
+    <row r="47" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N47" s="2"/>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N51" s="2"/>
+    </row>
+    <row r="55" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N55" s="1"/>
+    </row>
+    <row r="59" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N59" s="1"/>
+    </row>
+    <row r="63" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N63" s="1"/>
+    </row>
+    <row r="67" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N67" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>